<commit_message>
Setup Common Business Scenarios of Advanced Formula Action In No Time
Setup Common Business Scenarios of Advanced Formula Action In No Time
</commit_message>
<xml_diff>
--- a/AdvancedFormulaActionCommonScenarios/AggregateDimension.xlsx
+++ b/AdvancedFormulaActionCommonScenarios/AggregateDimension.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SAP\Blogs\Setup Common Business Scenarios of Advanced Formula Action In No Time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UladzislauP\Documents\GitHub\SAC\AdvancedFormulaActionCommonScenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDB3B99-164B-41AB-A368-92BFFB84BBCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3AF4F-9A64-45E0-806A-5E2A0E4CC8C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="4740" windowWidth="27510" windowHeight="14850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Transactional Data" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>ACC1</t>
   </si>
@@ -98,6 +99,57 @@
   </si>
   <si>
     <t>Data</t>
+  </si>
+  <si>
+    <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Account Type</t>
+  </si>
+  <si>
+    <t>Calculated On</t>
+  </si>
+  <si>
+    <t>Aggregation Type</t>
+  </si>
+  <si>
+    <t>Excepion Aggregation Type</t>
+  </si>
+  <si>
+    <t>Exception Aggregation Dimension</t>
+  </si>
+  <si>
+    <t>Required Dimensions</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Decimal Places</t>
+  </si>
+  <si>
+    <t>Units &amp; Currencies</t>
+  </si>
+  <si>
+    <t>Thresholds</t>
+  </si>
+  <si>
+    <t>Hide</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>&lt;root&gt;</t>
+  </si>
+  <si>
+    <t>NFIN</t>
+  </si>
+  <si>
+    <t>SUM</t>
   </si>
 </sst>
 </file>
@@ -536,10 +588,110 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BEB6F-9B2C-42E1-BEDC-C08DFFF884D4}">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Learn Advanced Formula Actions for Common Business Scenarios In No Time
Learn Advanced Formula Actions for Common Business Scenarios In No Time
</commit_message>
<xml_diff>
--- a/AdvancedFormulaActionCommonScenarios/AggregateDimension.xlsx
+++ b/AdvancedFormulaActionCommonScenarios/AggregateDimension.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UladzislauP\Documents\GitHub\SAC\AdvancedFormulaActionCommonScenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3AF4F-9A64-45E0-806A-5E2A0E4CC8C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C44DA5-606E-4CFE-8221-7789AF6EC07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="4740" windowWidth="27510" windowHeight="14850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="2" r:id="rId1"/>
@@ -478,9 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776AD500-EC84-4017-9AA5-4F62DBDDA14A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -591,9 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BEB6F-9B2C-42E1-BEDC-C08DFFF884D4}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -691,9 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>